<commit_message>
912 work by Alex
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhack/git/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE83848-199A-3D42-8139-C01F2EC2EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34415B06-1699-8446-BAD7-B29971236032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
   <si>
     <t>First Name</t>
   </si>
@@ -1352,6 +1352,15 @@
   </si>
   <si>
     <t>Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Race Unknown</t>
+  </si>
+  <si>
+    <t>Race Other</t>
+  </si>
+  <si>
+    <t>Race Refused to Answer</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CI4" sqref="CI4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CO1" workbookViewId="0">
+      <selection activeCell="CW5" sqref="CW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1809,9 +1818,13 @@
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="24" customWidth="1"/>
+    <col min="100" max="100" width="15.33203125" customWidth="1"/>
+    <col min="101" max="101" width="16" customWidth="1"/>
+    <col min="102" max="103" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2109,8 +2122,17 @@
       <c r="CU1" t="s">
         <v>443</v>
       </c>
+      <c r="CV1" t="s">
+        <v>444</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>445</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>446</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2391,7 +2413,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2672,7 +2694,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2953,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3189,7 +3211,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3443,7 +3465,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3700,7 +3722,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3957,7 +3979,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4238,7 +4260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4519,7 +4541,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4776,7 +4798,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
fixed the import problem, want to do one final check
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhack/git/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE83848-199A-3D42-8139-C01F2EC2EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34415B06-1699-8446-BAD7-B29971236032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
   <si>
     <t>First Name</t>
   </si>
@@ -1352,6 +1352,15 @@
   </si>
   <si>
     <t>Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Race Unknown</t>
+  </si>
+  <si>
+    <t>Race Other</t>
+  </si>
+  <si>
+    <t>Race Refused to Answer</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CI4" sqref="CI4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CO1" workbookViewId="0">
+      <selection activeCell="CW5" sqref="CW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1809,9 +1818,13 @@
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="24" customWidth="1"/>
+    <col min="100" max="100" width="15.33203125" customWidth="1"/>
+    <col min="101" max="101" width="16" customWidth="1"/>
+    <col min="102" max="103" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2109,8 +2122,17 @@
       <c r="CU1" t="s">
         <v>443</v>
       </c>
+      <c r="CV1" t="s">
+        <v>444</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>445</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>446</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2391,7 +2413,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2672,7 +2694,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2953,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3189,7 +3211,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3443,7 +3465,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3700,7 +3722,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3957,7 +3979,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4238,7 +4260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4519,7 +4541,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4776,7 +4798,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
readded excel conflicts, can be manually merged
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhack/git/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE83848-199A-3D42-8139-C01F2EC2EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34415B06-1699-8446-BAD7-B29971236032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
   <si>
     <t>First Name</t>
   </si>
@@ -1352,6 +1352,15 @@
   </si>
   <si>
     <t>Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Race Unknown</t>
+  </si>
+  <si>
+    <t>Race Other</t>
+  </si>
+  <si>
+    <t>Race Refused to Answer</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CI4" sqref="CI4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CO1" workbookViewId="0">
+      <selection activeCell="CW5" sqref="CW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1809,9 +1818,13 @@
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="24" customWidth="1"/>
+    <col min="100" max="100" width="15.33203125" customWidth="1"/>
+    <col min="101" max="101" width="16" customWidth="1"/>
+    <col min="102" max="103" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2109,8 +2122,17 @@
       <c r="CU1" t="s">
         <v>443</v>
       </c>
+      <c r="CV1" t="s">
+        <v>444</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>445</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>446</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2391,7 +2413,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2672,7 +2694,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2953,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3189,7 +3211,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3443,7 +3465,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3700,7 +3722,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3957,7 +3979,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4238,7 +4260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4519,7 +4541,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4776,7 +4798,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
add new race options to import/export , reorder race options for consistency, update excel files
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34415B06-1699-8446-BAD7-B29971236032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570BDC4-1CB0-5743-A4A4-174171637962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1715,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CO1" workbookViewId="0">
-      <selection activeCell="CW5" sqref="CW5"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CR1" workbookViewId="0">
+      <selection activeCell="CX4" sqref="CX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1803,11 +1803,11 @@
     <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="11.5" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="16" bestFit="1" customWidth="1"/>
@@ -1817,11 +1817,13 @@
     <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="24" customWidth="1"/>
-    <col min="100" max="100" width="15.33203125" customWidth="1"/>
-    <col min="101" max="101" width="16" customWidth="1"/>
-    <col min="102" max="103" width="22.6640625" customWidth="1"/>
+    <col min="97" max="97" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.15">
@@ -2123,10 +2125,10 @@
         <v>443</v>
       </c>
       <c r="CV1" t="s">
+        <v>445</v>
+      </c>
+      <c r="CW1" t="s">
         <v>444</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>445</v>
       </c>
       <c r="CX1" t="s">
         <v>446</v>

</xml_diff>

<commit_message>
allow vaccine table to be populated on import
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570BDC4-1CB0-5743-A4A4-174171637962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A403CBF-D186-794E-B499-5A8A1B14654B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10120" yWindow="2140" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="470">
   <si>
     <t>First Name</t>
   </si>
@@ -1361,6 +1361,75 @@
   </si>
   <si>
     <t>Race Refused to Answer</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Group Name</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Product Name</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Administration Date</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Dose Number</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Group Name</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Product Name</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Administration Date</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Dose Number</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Notes</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Notes</t>
+  </si>
+  <si>
+    <t>COVID-19</t>
+  </si>
+  <si>
+    <t>Moderna COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>2020-06-01</t>
+  </si>
+  <si>
+    <t>2020-06-20</t>
+  </si>
+  <si>
+    <t>notes 1</t>
+  </si>
+  <si>
+    <t>notes 2</t>
+  </si>
+  <si>
+    <t>Janssen (J&amp;J) COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>Pfizer-BioNTech COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>2020-06-02</t>
+  </si>
+  <si>
+    <t>2020-06-03</t>
+  </si>
+  <si>
+    <t>2020-06-04</t>
+  </si>
+  <si>
+    <t>2020-06-21</t>
+  </si>
+  <si>
+    <t>2020-06-22</t>
   </si>
 </sst>
 </file>
@@ -1713,11 +1782,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CX12"/>
+  <dimension ref="A1:DH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CR1" workbookViewId="0">
-      <selection activeCell="CX4" sqref="CX4"/>
-    </sheetView>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1823,10 +1890,19 @@
     <col min="100" max="100" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="22.6640625" customWidth="1"/>
+    <col min="103" max="103" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="31" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="31" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2133,8 +2209,38 @@
       <c r="CX1" t="s">
         <v>446</v>
       </c>
+      <c r="CY1" t="s">
+        <v>447</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>448</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>450</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>456</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>451</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>452</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>454</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>455</v>
+      </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2414,8 +2520,38 @@
       <c r="CS2">
         <v>378</v>
       </c>
+      <c r="CY2" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>458</v>
+      </c>
+      <c r="DA2" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="DB2">
+        <v>1</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>461</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>457</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>458</v>
+      </c>
+      <c r="DF2" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="DG2">
+        <v>2</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>462</v>
+      </c>
     </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2695,8 +2831,32 @@
       <c r="CQ3" t="s">
         <v>93</v>
       </c>
+      <c r="CY3" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>464</v>
+      </c>
+      <c r="DA3" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="DB3">
+        <v>1</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>457</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>464</v>
+      </c>
+      <c r="DF3" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="DG3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2976,8 +3136,32 @@
       <c r="CS4">
         <v>2</v>
       </c>
+      <c r="CY4" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ4" t="s">
+        <v>381</v>
+      </c>
+      <c r="DA4" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="DB4">
+        <v>1</v>
+      </c>
+      <c r="DD4" t="s">
+        <v>457</v>
+      </c>
+      <c r="DE4" t="s">
+        <v>381</v>
+      </c>
+      <c r="DF4" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="DG4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3212,8 +3396,20 @@
       <c r="CS5">
         <v>83</v>
       </c>
+      <c r="CY5" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ5" t="s">
+        <v>458</v>
+      </c>
+      <c r="DA5" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="DB5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3466,8 +3662,20 @@
       <c r="CS6">
         <v>83</v>
       </c>
+      <c r="CY6" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ6" t="s">
+        <v>463</v>
+      </c>
+      <c r="DA6" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="DB6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3723,8 +3931,20 @@
       <c r="CQ7" t="s">
         <v>320</v>
       </c>
+      <c r="CY7" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ7" t="s">
+        <v>381</v>
+      </c>
+      <c r="DA7" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="DB7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3981,7 +4201,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4262,7 +4482,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4543,7 +4763,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4800,7 +5020,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
SARAALERT-1260: Allow vaccine table to be populated on import (#958)
* allow vaccine table to be populated on import

* normalize vaccine enums

* fix import tests
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570BDC4-1CB0-5743-A4A4-174171637962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C885723B-7DF2-E748-80C7-6A6445D63090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10120" yWindow="2140" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="473">
   <si>
     <t>First Name</t>
   </si>
@@ -1361,6 +1361,84 @@
   </si>
   <si>
     <t>Race Refused to Answer</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Group Name</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Product Name</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Administration Date</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Dose Number</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Group Name</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Product Name</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Administration Date</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Dose Number</t>
+  </si>
+  <si>
+    <t>Vaccine 2 Notes</t>
+  </si>
+  <si>
+    <t>Vaccine 1 Notes</t>
+  </si>
+  <si>
+    <t>COVID-19</t>
+  </si>
+  <si>
+    <t>Moderna COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>2020-06-01</t>
+  </si>
+  <si>
+    <t>2020-06-20</t>
+  </si>
+  <si>
+    <t>notes 1</t>
+  </si>
+  <si>
+    <t>notes 2</t>
+  </si>
+  <si>
+    <t>Janssen (J&amp;J) COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>Pfizer-BioNTech COVID-19 Vaccine</t>
+  </si>
+  <si>
+    <t>2020-06-02</t>
+  </si>
+  <si>
+    <t>2020-06-03</t>
+  </si>
+  <si>
+    <t>2020-06-04</t>
+  </si>
+  <si>
+    <t>2020-06-21</t>
+  </si>
+  <si>
+    <t>2020-06-22</t>
+  </si>
+  <si>
+    <t>covid19</t>
+  </si>
+  <si>
+    <t>moderna covid19 vaccine</t>
+  </si>
+  <si>
+    <t>pfizerbiontech covid19 vaccine</t>
   </si>
 </sst>
 </file>
@@ -1713,11 +1791,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CX12"/>
+  <dimension ref="A1:DH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CR1" workbookViewId="0">
-      <selection activeCell="CX4" sqref="CX4"/>
-    </sheetView>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1823,10 +1899,19 @@
     <col min="100" max="100" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="22.6640625" customWidth="1"/>
+    <col min="103" max="103" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="31" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="31" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2133,8 +2218,38 @@
       <c r="CX1" t="s">
         <v>446</v>
       </c>
+      <c r="CY1" t="s">
+        <v>447</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>448</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>450</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>456</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>451</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>452</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>454</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>455</v>
+      </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2414,8 +2529,38 @@
       <c r="CS2">
         <v>378</v>
       </c>
+      <c r="CY2" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>458</v>
+      </c>
+      <c r="DA2" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="DB2">
+        <v>1</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>461</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>470</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>471</v>
+      </c>
+      <c r="DF2" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="DG2">
+        <v>2</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>462</v>
+      </c>
     </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2695,8 +2840,32 @@
       <c r="CQ3" t="s">
         <v>93</v>
       </c>
+      <c r="CY3" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>464</v>
+      </c>
+      <c r="DA3" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="DB3">
+        <v>1</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>457</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>472</v>
+      </c>
+      <c r="DF3" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="DG3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2976,8 +3145,32 @@
       <c r="CS4">
         <v>2</v>
       </c>
+      <c r="CY4" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ4" t="s">
+        <v>381</v>
+      </c>
+      <c r="DA4" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="DB4">
+        <v>1</v>
+      </c>
+      <c r="DD4" t="s">
+        <v>457</v>
+      </c>
+      <c r="DE4" t="s">
+        <v>438</v>
+      </c>
+      <c r="DF4" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="DG4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3212,8 +3405,20 @@
       <c r="CS5">
         <v>83</v>
       </c>
+      <c r="CY5" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ5" t="s">
+        <v>458</v>
+      </c>
+      <c r="DA5" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="DB5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3466,8 +3671,20 @@
       <c r="CS6">
         <v>83</v>
       </c>
+      <c r="CY6" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ6" t="s">
+        <v>463</v>
+      </c>
+      <c r="DA6" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="DB6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3723,8 +3940,20 @@
       <c r="CQ7" t="s">
         <v>320</v>
       </c>
+      <c r="CY7" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ7" t="s">
+        <v>381</v>
+      </c>
+      <c r="DA7" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="DB7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3981,7 +4210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4262,7 +4491,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4543,7 +4772,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4800,7 +5029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
add follow-up fields to import/export and include first_positive_lab in canned exports
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C885723B-7DF2-E748-80C7-6A6445D63090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF7CD85-5FB5-3847-B3AC-B2ECAE229887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="2140" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="478">
   <si>
     <t>First Name</t>
   </si>
@@ -1439,6 +1439,21 @@
   </si>
   <si>
     <t>pfizerbiontech covid19 vaccine</t>
+  </si>
+  <si>
+    <t>Follow-Up Reason</t>
+  </si>
+  <si>
+    <t>Follow-Up Note</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Hospitalized</t>
+  </si>
+  <si>
+    <t>example note</t>
   </si>
 </sst>
 </file>
@@ -1791,7 +1806,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DH12"/>
+  <dimension ref="A1:DJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
@@ -1909,9 +1924,11 @@
     <col min="110" max="110" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2248,8 +2265,14 @@
       <c r="DH1" t="s">
         <v>455</v>
       </c>
+      <c r="DI1" t="s">
+        <v>473</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>474</v>
+      </c>
     </row>
-    <row r="2" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2559,8 +2582,14 @@
       <c r="DH2" t="s">
         <v>462</v>
       </c>
+      <c r="DI2" t="s">
+        <v>475</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="3" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2864,8 +2893,11 @@
       <c r="DG3">
         <v>2</v>
       </c>
+      <c r="DI3" t="s">
+        <v>476</v>
+      </c>
     </row>
-    <row r="4" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -3170,7 +3202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3418,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3684,7 +3716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3953,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -4210,7 +4242,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4491,7 +4523,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4772,7 +4804,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -5029,7 +5061,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
SARAALERT-1521: Import/export follow-up fields (#983)
* add follow-up fields to import/export and include first_positive_lab in canned exports

* validate follow_up_note and update formatting guidance release date

* add patient tests

* validate follow_up_reason instead of follow_up_note
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C885723B-7DF2-E748-80C7-6A6445D63090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF7CD85-5FB5-3847-B3AC-B2ECAE229887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="2140" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="478">
   <si>
     <t>First Name</t>
   </si>
@@ -1439,6 +1439,21 @@
   </si>
   <si>
     <t>pfizerbiontech covid19 vaccine</t>
+  </si>
+  <si>
+    <t>Follow-Up Reason</t>
+  </si>
+  <si>
+    <t>Follow-Up Note</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Hospitalized</t>
+  </si>
+  <si>
+    <t>example note</t>
   </si>
 </sst>
 </file>
@@ -1791,7 +1806,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DH12"/>
+  <dimension ref="A1:DJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
@@ -1909,9 +1924,11 @@
     <col min="110" max="110" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2248,8 +2265,14 @@
       <c r="DH1" t="s">
         <v>455</v>
       </c>
+      <c r="DI1" t="s">
+        <v>473</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>474</v>
+      </c>
     </row>
-    <row r="2" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2559,8 +2582,14 @@
       <c r="DH2" t="s">
         <v>462</v>
       </c>
+      <c r="DI2" t="s">
+        <v>475</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="3" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2864,8 +2893,11 @@
       <c r="DG3">
         <v>2</v>
       </c>
+      <c r="DI3" t="s">
+        <v>476</v>
+      </c>
     </row>
-    <row r="4" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -3170,7 +3202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3418,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3684,7 +3716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3953,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -4210,7 +4242,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4491,7 +4523,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4772,7 +4804,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -5029,7 +5061,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:112" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
Revert "1.34 Candidate (#979)"
This reverts commit d0870011ae9ecf36c112cb319516646f3626a21c.
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF7CD85-5FB5-3847-B3AC-B2ECAE229887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C885723B-7DF2-E748-80C7-6A6445D63090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10120" yWindow="2140" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="473">
   <si>
     <t>First Name</t>
   </si>
@@ -1439,21 +1439,6 @@
   </si>
   <si>
     <t>pfizerbiontech covid19 vaccine</t>
-  </si>
-  <si>
-    <t>Follow-Up Reason</t>
-  </si>
-  <si>
-    <t>Follow-Up Note</t>
-  </si>
-  <si>
-    <t>Duplicate</t>
-  </si>
-  <si>
-    <t>Hospitalized</t>
-  </si>
-  <si>
-    <t>example note</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1791,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DJ12"/>
+  <dimension ref="A1:DH12"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
@@ -1924,11 +1909,9 @@
     <col min="110" max="110" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2265,14 +2248,8 @@
       <c r="DH1" t="s">
         <v>455</v>
       </c>
-      <c r="DI1" t="s">
-        <v>473</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>474</v>
-      </c>
     </row>
-    <row r="2" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2582,14 +2559,8 @@
       <c r="DH2" t="s">
         <v>462</v>
       </c>
-      <c r="DI2" t="s">
-        <v>475</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>477</v>
-      </c>
     </row>
-    <row r="3" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2893,11 +2864,8 @@
       <c r="DG3">
         <v>2</v>
       </c>
-      <c r="DI3" t="s">
-        <v>476</v>
-      </c>
     </row>
-    <row r="4" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -3202,7 +3170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3450,7 +3418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3716,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3985,7 +3953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -4242,7 +4210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4523,7 +4491,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4804,7 +4772,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -5061,7 +5029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:114" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:112" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
fix preferred contact time validation options
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfagan/Documents/Projects/CDC/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F4EED-A92B-BF42-A1AB-1D4495336031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F62D0C-76EF-A448-861E-82C19732B087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="481">
   <si>
     <t>First Name</t>
   </si>
@@ -1273,18 +1273,6 @@
     <t>MORNING</t>
   </si>
   <si>
-    <t>mor ning</t>
-  </si>
-  <si>
-    <t>after-nOON</t>
-  </si>
-  <si>
-    <t>eve ning</t>
-  </si>
-  <si>
-    <t>EVENinG</t>
-  </si>
-  <si>
     <t>international</t>
   </si>
   <si>
@@ -1454,6 +1442,24 @@
   </si>
   <si>
     <t>example note</t>
+  </si>
+  <si>
+    <t>MIDNIGHT</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>midnight</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>evening</t>
   </si>
   <si>
     <t>AstraZeneca COVID-19 Vaccine (non-US)</t>
@@ -1811,9 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CZ1" workbookViewId="0">
-      <selection activeCell="CZ1" sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1865,7 +1869,7 @@
     <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -2078,7 +2082,7 @@
       <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="AX1" t="s">
@@ -2226,55 +2230,55 @@
         <v>386</v>
       </c>
       <c r="CT1" t="s">
+        <v>438</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>439</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>441</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>440</v>
+      </c>
+      <c r="CX1" t="s">
         <v>442</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CY1" t="s">
         <v>443</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CZ1" t="s">
+        <v>444</v>
+      </c>
+      <c r="DA1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="CW1" t="s">
-        <v>444</v>
-      </c>
-      <c r="CX1" t="s">
+      <c r="DB1" t="s">
         <v>446</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DC1" t="s">
+        <v>452</v>
+      </c>
+      <c r="DD1" t="s">
         <v>447</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DE1" t="s">
         <v>448</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DG1" t="s">
         <v>450</v>
       </c>
-      <c r="DC1" t="s">
-        <v>456</v>
-      </c>
-      <c r="DD1" t="s">
+      <c r="DH1" t="s">
         <v>451</v>
       </c>
-      <c r="DE1" t="s">
-        <v>452</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>454</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>455</v>
-      </c>
       <c r="DI1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="DJ1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:114" x14ac:dyDescent="0.15">
@@ -2422,7 +2426,7 @@
       <c r="AV2" t="s">
         <v>103</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="1" t="s">
         <v>416</v>
       </c>
       <c r="AX2" t="s">
@@ -2453,7 +2457,7 @@
         <v>93</v>
       </c>
       <c r="BG2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="BH2" t="s">
         <v>93</v>
@@ -2525,7 +2529,7 @@
         <v>115</v>
       </c>
       <c r="CE2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="CF2" t="s">
         <v>93</v>
@@ -2558,40 +2562,40 @@
         <v>378</v>
       </c>
       <c r="CY2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="DB2">
         <v>1</v>
       </c>
       <c r="DC2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="DD2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="DE2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="DG2">
         <v>2</v>
       </c>
       <c r="DH2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="DI2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="DJ2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:114" x14ac:dyDescent="0.15">
@@ -2736,7 +2740,7 @@
       <c r="AV3" t="s">
         <v>414</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3" s="1" t="s">
         <v>415</v>
       </c>
       <c r="AX3" t="s">
@@ -2839,7 +2843,7 @@
         <v>140</v>
       </c>
       <c r="CE3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="CF3" t="s">
         <v>332</v>
@@ -2875,31 +2879,31 @@
         <v>93</v>
       </c>
       <c r="CY3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ3" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="DA3" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="DB3">
         <v>1</v>
       </c>
       <c r="DD3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="DE3" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="DF3" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="DG3">
         <v>2</v>
       </c>
       <c r="DI3" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:114" x14ac:dyDescent="0.15">
@@ -3044,8 +3048,8 @@
       <c r="AV4" t="s">
         <v>409</v>
       </c>
-      <c r="AW4" t="s">
-        <v>417</v>
+      <c r="AW4" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="AX4" t="s">
         <v>155</v>
@@ -3075,7 +3079,7 @@
         <v>93</v>
       </c>
       <c r="BG4" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="BH4" t="s">
         <v>93</v>
@@ -3141,7 +3145,7 @@
         <v>93</v>
       </c>
       <c r="CD4" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="CE4" t="s">
         <v>141</v>
@@ -3183,25 +3187,25 @@
         <v>2</v>
       </c>
       <c r="CY4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ4" t="s">
         <v>381</v>
       </c>
       <c r="DA4" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="DB4">
         <v>1</v>
       </c>
       <c r="DD4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="DE4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="DF4" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="DG4">
         <v>2</v>
@@ -3352,7 +3356,7 @@
       <c r="AV5" t="s">
         <v>103</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5" s="1" t="s">
         <v>353</v>
       </c>
       <c r="AX5" t="s">
@@ -3362,7 +3366,7 @@
         <v>377</v>
       </c>
       <c r="BG5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="BI5" t="s">
         <v>93</v>
@@ -3443,13 +3447,13 @@
         <v>83</v>
       </c>
       <c r="CY5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="DA5" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="DB5">
         <v>1</v>
@@ -3580,7 +3584,7 @@
         <v>103</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>418</v>
+        <v>478</v>
       </c>
       <c r="AX6" t="s">
         <v>187</v>
@@ -3691,7 +3695,7 @@
         <v>322</v>
       </c>
       <c r="CI6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="CJ6" t="s">
         <v>323</v>
@@ -3709,13 +3713,13 @@
         <v>83</v>
       </c>
       <c r="CY6" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="DA6" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="DB6">
         <v>1</v>
@@ -3842,7 +3846,7 @@
       <c r="AV7" t="s">
         <v>410</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AW7" s="1" t="s">
         <v>354</v>
       </c>
       <c r="AX7" t="s">
@@ -3873,7 +3877,7 @@
         <v>93</v>
       </c>
       <c r="BG7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="BH7" t="s">
         <v>212</v>
@@ -3939,10 +3943,10 @@
         <v>336</v>
       </c>
       <c r="CD7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="CE7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="CF7" t="s">
         <v>93</v>
@@ -3978,13 +3982,13 @@
         <v>320</v>
       </c>
       <c r="CY7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ7" t="s">
         <v>381</v>
       </c>
       <c r="DA7" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="DB7">
         <v>1</v>
@@ -4135,8 +4139,8 @@
       <c r="AV8" t="s">
         <v>103</v>
       </c>
-      <c r="AW8" t="s">
-        <v>419</v>
+      <c r="AW8" s="1" t="s">
+        <v>479</v>
       </c>
       <c r="AX8" t="s">
         <v>228</v>
@@ -4166,7 +4170,7 @@
         <v>93</v>
       </c>
       <c r="BG8" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="BH8" t="s">
         <v>93</v>
@@ -4238,7 +4242,7 @@
         <v>380</v>
       </c>
       <c r="CE8" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="CF8" t="s">
         <v>93</v>
@@ -4247,13 +4251,13 @@
         <v>57</v>
       </c>
       <c r="CY8" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="DA8" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="DB8">
         <v>1</v>
@@ -4404,8 +4408,8 @@
       <c r="AV9" t="s">
         <v>411</v>
       </c>
-      <c r="AW9" t="s">
-        <v>420</v>
+      <c r="AW9" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="AX9" t="s">
         <v>244</v>
@@ -4504,16 +4508,16 @@
         <v>338</v>
       </c>
       <c r="CD9" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="CE9" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="CF9" t="s">
         <v>334</v>
       </c>
       <c r="CI9" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="CJ9" t="s">
         <v>93</v>
@@ -4685,8 +4689,8 @@
       <c r="AV10" t="s">
         <v>103</v>
       </c>
-      <c r="AW10" t="s">
-        <v>93</v>
+      <c r="AW10" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="AX10" t="s">
         <v>264</v>
@@ -4779,10 +4783,10 @@
         <v>89</v>
       </c>
       <c r="CD10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="CE10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="CF10" t="s">
         <v>93</v>
@@ -4939,8 +4943,8 @@
       <c r="AV11" t="s">
         <v>412</v>
       </c>
-      <c r="AW11" t="s">
-        <v>93</v>
+      <c r="AW11" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="AX11" t="s">
         <v>280</v>
@@ -5036,10 +5040,10 @@
         <v>93</v>
       </c>
       <c r="CD11" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="CE11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="CF11" t="s">
         <v>335</v>
@@ -5051,7 +5055,7 @@
         <v>93</v>
       </c>
       <c r="CI11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="CJ11" t="s">
         <v>93</v>
@@ -5176,7 +5180,7 @@
         <v>318</v>
       </c>
       <c r="CI12" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="CJ12" t="s">
         <v>321</v>

</xml_diff>

<commit_message>
Add AstraZeneca vaccine to configuration   * config/vaccines.yml   * Import format   * Advanced filter   * System test file fixtures
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfagan/Documents/Projects/CDC/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF7CD85-5FB5-3847-B3AC-B2ECAE229887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F4EED-A92B-BF42-A1AB-1D4495336031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="479">
   <si>
     <t>First Name</t>
   </si>
@@ -1454,6 +1454,9 @@
   </si>
   <si>
     <t>example note</t>
+  </si>
+  <si>
+    <t>AstraZeneca COVID-19 Vaccine (non-US)</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CZ1" workbookViewId="0">
+      <selection activeCell="CZ1" sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4241,6 +4246,18 @@
       <c r="CS8">
         <v>57</v>
       </c>
+      <c r="CY8" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ8" t="s">
+        <v>478</v>
+      </c>
+      <c r="DA8" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="DB8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
SARAALERT-1542: Add AstraZeneca vaccine to configuration (#1033)
* Add AstraZeneca vaccine to configuration
  * config/vaccines.yml
  * Import format
  * Advanced filter
  * System test file fixtures

* Change updated at date of the import guidance
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfagan/Documents/Projects/CDC/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF7CD85-5FB5-3847-B3AC-B2ECAE229887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F4EED-A92B-BF42-A1AB-1D4495336031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="479">
   <si>
     <t>First Name</t>
   </si>
@@ -1454,6 +1454,9 @@
   </si>
   <si>
     <t>example note</t>
+  </si>
+  <si>
+    <t>AstraZeneca COVID-19 Vaccine (non-US)</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CZ1" workbookViewId="0">
+      <selection activeCell="CZ1" sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4241,6 +4246,18 @@
       <c r="CS8">
         <v>57</v>
       </c>
+      <c r="CY8" t="s">
+        <v>457</v>
+      </c>
+      <c r="CZ8" t="s">
+        <v>478</v>
+      </c>
+      <c r="DA8" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="DB8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
SARAALERT-513: Customize timing of daily reports (#1019)
* add custom preferred contact time

* use formatted preferred contact times for import/export and format select input

* update test fixtures with more edge cases

* extend time window for contacting patients

* address PR comments from Nick

* pad hours with leading 0

* fix preferred contact time validation options

* add min height to react select options
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfagan/Documents/Projects/CDC/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F4EED-A92B-BF42-A1AB-1D4495336031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F62D0C-76EF-A448-861E-82C19732B087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="481">
   <si>
     <t>First Name</t>
   </si>
@@ -1273,18 +1273,6 @@
     <t>MORNING</t>
   </si>
   <si>
-    <t>mor ning</t>
-  </si>
-  <si>
-    <t>after-nOON</t>
-  </si>
-  <si>
-    <t>eve ning</t>
-  </si>
-  <si>
-    <t>EVENinG</t>
-  </si>
-  <si>
     <t>international</t>
   </si>
   <si>
@@ -1454,6 +1442,24 @@
   </si>
   <si>
     <t>example note</t>
+  </si>
+  <si>
+    <t>MIDNIGHT</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>midnight</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>evening</t>
   </si>
   <si>
     <t>AstraZeneca COVID-19 Vaccine (non-US)</t>
@@ -1811,9 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CZ1" workbookViewId="0">
-      <selection activeCell="CZ1" sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1865,7 +1869,7 @@
     <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -2078,7 +2082,7 @@
       <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="AX1" t="s">
@@ -2226,55 +2230,55 @@
         <v>386</v>
       </c>
       <c r="CT1" t="s">
+        <v>438</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>439</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>441</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>440</v>
+      </c>
+      <c r="CX1" t="s">
         <v>442</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CY1" t="s">
         <v>443</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CZ1" t="s">
+        <v>444</v>
+      </c>
+      <c r="DA1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="CW1" t="s">
-        <v>444</v>
-      </c>
-      <c r="CX1" t="s">
+      <c r="DB1" t="s">
         <v>446</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DC1" t="s">
+        <v>452</v>
+      </c>
+      <c r="DD1" t="s">
         <v>447</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DE1" t="s">
         <v>448</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DG1" t="s">
         <v>450</v>
       </c>
-      <c r="DC1" t="s">
-        <v>456</v>
-      </c>
-      <c r="DD1" t="s">
+      <c r="DH1" t="s">
         <v>451</v>
       </c>
-      <c r="DE1" t="s">
-        <v>452</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>454</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>455</v>
-      </c>
       <c r="DI1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="DJ1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:114" x14ac:dyDescent="0.15">
@@ -2422,7 +2426,7 @@
       <c r="AV2" t="s">
         <v>103</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="1" t="s">
         <v>416</v>
       </c>
       <c r="AX2" t="s">
@@ -2453,7 +2457,7 @@
         <v>93</v>
       </c>
       <c r="BG2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="BH2" t="s">
         <v>93</v>
@@ -2525,7 +2529,7 @@
         <v>115</v>
       </c>
       <c r="CE2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="CF2" t="s">
         <v>93</v>
@@ -2558,40 +2562,40 @@
         <v>378</v>
       </c>
       <c r="CY2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="DB2">
         <v>1</v>
       </c>
       <c r="DC2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="DD2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="DE2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="DG2">
         <v>2</v>
       </c>
       <c r="DH2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="DI2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="DJ2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:114" x14ac:dyDescent="0.15">
@@ -2736,7 +2740,7 @@
       <c r="AV3" t="s">
         <v>414</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3" s="1" t="s">
         <v>415</v>
       </c>
       <c r="AX3" t="s">
@@ -2839,7 +2843,7 @@
         <v>140</v>
       </c>
       <c r="CE3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="CF3" t="s">
         <v>332</v>
@@ -2875,31 +2879,31 @@
         <v>93</v>
       </c>
       <c r="CY3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ3" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="DA3" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="DB3">
         <v>1</v>
       </c>
       <c r="DD3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="DE3" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="DF3" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="DG3">
         <v>2</v>
       </c>
       <c r="DI3" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:114" x14ac:dyDescent="0.15">
@@ -3044,8 +3048,8 @@
       <c r="AV4" t="s">
         <v>409</v>
       </c>
-      <c r="AW4" t="s">
-        <v>417</v>
+      <c r="AW4" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="AX4" t="s">
         <v>155</v>
@@ -3075,7 +3079,7 @@
         <v>93</v>
       </c>
       <c r="BG4" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="BH4" t="s">
         <v>93</v>
@@ -3141,7 +3145,7 @@
         <v>93</v>
       </c>
       <c r="CD4" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="CE4" t="s">
         <v>141</v>
@@ -3183,25 +3187,25 @@
         <v>2</v>
       </c>
       <c r="CY4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ4" t="s">
         <v>381</v>
       </c>
       <c r="DA4" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="DB4">
         <v>1</v>
       </c>
       <c r="DD4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="DE4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="DF4" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="DG4">
         <v>2</v>
@@ -3352,7 +3356,7 @@
       <c r="AV5" t="s">
         <v>103</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5" s="1" t="s">
         <v>353</v>
       </c>
       <c r="AX5" t="s">
@@ -3362,7 +3366,7 @@
         <v>377</v>
       </c>
       <c r="BG5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="BI5" t="s">
         <v>93</v>
@@ -3443,13 +3447,13 @@
         <v>83</v>
       </c>
       <c r="CY5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="DA5" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="DB5">
         <v>1</v>
@@ -3580,7 +3584,7 @@
         <v>103</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>418</v>
+        <v>478</v>
       </c>
       <c r="AX6" t="s">
         <v>187</v>
@@ -3691,7 +3695,7 @@
         <v>322</v>
       </c>
       <c r="CI6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="CJ6" t="s">
         <v>323</v>
@@ -3709,13 +3713,13 @@
         <v>83</v>
       </c>
       <c r="CY6" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="DA6" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="DB6">
         <v>1</v>
@@ -3842,7 +3846,7 @@
       <c r="AV7" t="s">
         <v>410</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AW7" s="1" t="s">
         <v>354</v>
       </c>
       <c r="AX7" t="s">
@@ -3873,7 +3877,7 @@
         <v>93</v>
       </c>
       <c r="BG7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="BH7" t="s">
         <v>212</v>
@@ -3939,10 +3943,10 @@
         <v>336</v>
       </c>
       <c r="CD7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="CE7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="CF7" t="s">
         <v>93</v>
@@ -3978,13 +3982,13 @@
         <v>320</v>
       </c>
       <c r="CY7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ7" t="s">
         <v>381</v>
       </c>
       <c r="DA7" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="DB7">
         <v>1</v>
@@ -4135,8 +4139,8 @@
       <c r="AV8" t="s">
         <v>103</v>
       </c>
-      <c r="AW8" t="s">
-        <v>419</v>
+      <c r="AW8" s="1" t="s">
+        <v>479</v>
       </c>
       <c r="AX8" t="s">
         <v>228</v>
@@ -4166,7 +4170,7 @@
         <v>93</v>
       </c>
       <c r="BG8" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="BH8" t="s">
         <v>93</v>
@@ -4238,7 +4242,7 @@
         <v>380</v>
       </c>
       <c r="CE8" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="CF8" t="s">
         <v>93</v>
@@ -4247,13 +4251,13 @@
         <v>57</v>
       </c>
       <c r="CY8" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="CZ8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="DA8" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="DB8">
         <v>1</v>
@@ -4404,8 +4408,8 @@
       <c r="AV9" t="s">
         <v>411</v>
       </c>
-      <c r="AW9" t="s">
-        <v>420</v>
+      <c r="AW9" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="AX9" t="s">
         <v>244</v>
@@ -4504,16 +4508,16 @@
         <v>338</v>
       </c>
       <c r="CD9" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="CE9" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="CF9" t="s">
         <v>334</v>
       </c>
       <c r="CI9" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="CJ9" t="s">
         <v>93</v>
@@ -4685,8 +4689,8 @@
       <c r="AV10" t="s">
         <v>103</v>
       </c>
-      <c r="AW10" t="s">
-        <v>93</v>
+      <c r="AW10" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="AX10" t="s">
         <v>264</v>
@@ -4779,10 +4783,10 @@
         <v>89</v>
       </c>
       <c r="CD10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="CE10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="CF10" t="s">
         <v>93</v>
@@ -4939,8 +4943,8 @@
       <c r="AV11" t="s">
         <v>412</v>
       </c>
-      <c r="AW11" t="s">
-        <v>93</v>
+      <c r="AW11" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="AX11" t="s">
         <v>280</v>
@@ -5036,10 +5040,10 @@
         <v>93</v>
       </c>
       <c r="CD11" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="CE11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="CF11" t="s">
         <v>335</v>
@@ -5051,7 +5055,7 @@
         <v>93</v>
       </c>
       <c r="CI11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="CJ11" t="s">
         <v>93</v>
@@ -5176,7 +5180,7 @@
         <v>318</v>
       </c>
       <c r="CI12" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="CJ12" t="s">
         <v>321</v>

</xml_diff>